<commit_message>
Creacion de los objetos DAO de las clases GrupoUsuario, Rol, RolGrupoUsuario, Sesion y Usuario
</commit_message>
<xml_diff>
--- a/Documentation/DataDictionary.xlsx
+++ b/Documentation/DataDictionary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.0.216\Ingenieria Software\Projects\Canadevi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Shift-F6\Proyectos\canadevi\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8B58688D-0986-4839-933C-25F533D7DD8B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C085E109-D990-4F13-84B6-17E210ADD608}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1611" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1613" uniqueCount="272">
   <si>
     <t>Collation:</t>
   </si>
@@ -457,9 +457,6 @@
     <t>Identificador del grupo de usuario</t>
   </si>
   <si>
-    <t>nombreGrupo</t>
-  </si>
-  <si>
     <t>Nombre del grupo de usuario</t>
   </si>
   <si>
@@ -730,24 +727,12 @@
     <t>Identificador de la sesión</t>
   </si>
   <si>
-    <t>fechaA</t>
-  </si>
-  <si>
     <t>Fecha en la que acceso al sistema</t>
   </si>
   <si>
-    <t>horaA</t>
-  </si>
-  <si>
     <t>Hora en la que acceso al sistema</t>
   </si>
   <si>
-    <t>fechaC</t>
-  </si>
-  <si>
-    <t>horaC</t>
-  </si>
-  <si>
     <t>Usuario  que acceso al sistema</t>
   </si>
   <si>
@@ -763,18 +748,12 @@
     <t>GRUPOUSUARIO</t>
   </si>
   <si>
-    <t>ROL</t>
-  </si>
-  <si>
     <t>ROLGRUPOUSUARIO</t>
   </si>
   <si>
     <t>TRAMITES</t>
   </si>
   <si>
-    <t>OFICIO</t>
-  </si>
-  <si>
     <t>SOLICITUDES</t>
   </si>
   <si>
@@ -848,6 +827,30 @@
   </si>
   <si>
     <t>C - Crear, A - Actualizar, E - Eliminar</t>
+  </si>
+  <si>
+    <t>Hora en la que se salio del sistema</t>
+  </si>
+  <si>
+    <t>Fecha en la que se salio del sistema</t>
+  </si>
+  <si>
+    <t>ROLES</t>
+  </si>
+  <si>
+    <t>OFICIOS</t>
+  </si>
+  <si>
+    <t>fechaApertura</t>
+  </si>
+  <si>
+    <t>horaApertura</t>
+  </si>
+  <si>
+    <t>fechaCierre</t>
+  </si>
+  <si>
+    <t>horaCierre</t>
   </si>
 </sst>
 </file>
@@ -1139,7 +1142,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -1244,6 +1247,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1310,7 +1316,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1656,7 +1662,7 @@
   <sheetData>
     <row r="1" spans="2:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H1" s="17" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
     </row>
     <row r="2" spans="2:13" s="17" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1676,20 +1682,20 @@
       <c r="M2" s="18"/>
     </row>
     <row r="3" spans="2:13" s="17" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="40" t="s">
-        <v>251</v>
-      </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="40"/>
+      <c r="B3" s="41" t="s">
+        <v>244</v>
+      </c>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
     </row>
     <row r="4" spans="2:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="18"/>
@@ -1722,32 +1728,32 @@
       <c r="M5" s="18"/>
     </row>
     <row r="6" spans="2:13" s="17" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="40" t="s">
-        <v>252</v>
-      </c>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="40"/>
-      <c r="J6" s="40"/>
-      <c r="K6" s="40"/>
-      <c r="L6" s="40"/>
-      <c r="M6" s="40"/>
+      <c r="B6" s="41" t="s">
+        <v>245</v>
+      </c>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="41"/>
     </row>
     <row r="7" spans="2:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="42"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
       <c r="J7" s="18"/>
       <c r="K7" s="18"/>
       <c r="L7" s="18"/>
@@ -1784,20 +1790,20 @@
       <c r="M9" s="18"/>
     </row>
     <row r="10" spans="2:13" s="17" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="40" t="s">
-        <v>253</v>
-      </c>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="40"/>
-      <c r="J10" s="40"/>
-      <c r="K10" s="40"/>
-      <c r="L10" s="40"/>
-      <c r="M10" s="40"/>
+      <c r="B10" s="41" t="s">
+        <v>246</v>
+      </c>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="41"/>
+      <c r="K10" s="41"/>
+      <c r="L10" s="41"/>
+      <c r="M10" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1859,19 +1865,19 @@
       <c r="O2" s="30"/>
     </row>
     <row r="3" spans="2:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="43"/>
-      <c r="N3" s="43"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="44"/>
       <c r="O3" s="30"/>
     </row>
     <row r="4" spans="2:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1965,8 +1971,8 @@
   </sheetPr>
   <dimension ref="A1:R158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Q146" sqref="Q146"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C158" sqref="C158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1998,7 +2004,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D2" s="36"/>
       <c r="E2" s="36"/>
@@ -2014,21 +2020,21 @@
       <c r="O2" s="30"/>
     </row>
     <row r="3" spans="1:18" s="17" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="43"/>
-      <c r="N3" s="43"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="44"/>
       <c r="O3" s="30"/>
     </row>
     <row r="4" spans="1:18" s="17" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2511,7 +2517,7 @@
     <row r="15" spans="1:18" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="26" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="C15" s="38" t="s">
         <v>37</v>
@@ -2777,7 +2783,7 @@
     <row r="21" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="26" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="C21" s="39" t="s">
         <v>47</v>
@@ -2830,7 +2836,7 @@
         <v>1</v>
       </c>
       <c r="C23" s="37" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="D23" s="18"/>
       <c r="E23" s="20"/>
@@ -2846,21 +2852,21 @@
       <c r="O23" s="30"/>
     </row>
     <row r="24" spans="1:15" s="17" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="43" t="s">
+      <c r="B24" s="44" t="s">
         <v>87</v>
       </c>
-      <c r="C24" s="43"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="43"/>
-      <c r="H24" s="43"/>
-      <c r="I24" s="43"/>
-      <c r="J24" s="43"/>
-      <c r="K24" s="43"/>
-      <c r="L24" s="43"/>
-      <c r="M24" s="43"/>
-      <c r="N24" s="43"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="44"/>
+      <c r="F24" s="44"/>
+      <c r="G24" s="44"/>
+      <c r="H24" s="44"/>
+      <c r="I24" s="44"/>
+      <c r="J24" s="44"/>
+      <c r="K24" s="44"/>
+      <c r="L24" s="44"/>
+      <c r="M24" s="44"/>
+      <c r="N24" s="44"/>
       <c r="O24" s="30"/>
     </row>
     <row r="25" spans="1:15" s="17" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3679,7 +3685,7 @@
     <row r="44" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
       <c r="B44" s="26" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="C44" s="38" t="s">
         <v>37</v>
@@ -3858,7 +3864,7 @@
         <v>1</v>
       </c>
       <c r="C49" s="37" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="D49" s="18"/>
       <c r="E49" s="20"/>
@@ -3874,21 +3880,21 @@
       <c r="O49" s="30"/>
     </row>
     <row r="50" spans="2:15" s="17" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="43" t="s">
+      <c r="B50" s="44" t="s">
         <v>124</v>
       </c>
-      <c r="C50" s="43"/>
-      <c r="D50" s="43"/>
-      <c r="E50" s="43"/>
-      <c r="F50" s="43"/>
-      <c r="G50" s="43"/>
-      <c r="H50" s="43"/>
-      <c r="I50" s="43"/>
-      <c r="J50" s="43"/>
-      <c r="K50" s="43"/>
-      <c r="L50" s="43"/>
-      <c r="M50" s="43"/>
-      <c r="N50" s="43"/>
+      <c r="C50" s="44"/>
+      <c r="D50" s="44"/>
+      <c r="E50" s="44"/>
+      <c r="F50" s="44"/>
+      <c r="G50" s="44"/>
+      <c r="H50" s="44"/>
+      <c r="I50" s="44"/>
+      <c r="J50" s="44"/>
+      <c r="K50" s="44"/>
+      <c r="L50" s="44"/>
+      <c r="M50" s="44"/>
+      <c r="N50" s="44"/>
       <c r="O50" s="30"/>
     </row>
     <row r="51" spans="2:15" s="17" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4024,7 +4030,7 @@
         <v>127</v>
       </c>
       <c r="C54" s="24" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="D54" s="24" t="s">
         <v>41</v>
@@ -4060,7 +4066,7 @@
         <v>36</v>
       </c>
       <c r="O54" s="24" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
     </row>
     <row r="55" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -4301,10 +4307,10 @@
       <c r="B61" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C61" s="44" t="s">
-        <v>241</v>
-      </c>
-      <c r="D61" s="44"/>
+      <c r="C61" s="45" t="s">
+        <v>236</v>
+      </c>
+      <c r="D61" s="45"/>
       <c r="E61" s="20"/>
       <c r="F61" s="18"/>
       <c r="G61" s="18"/>
@@ -4318,21 +4324,21 @@
       <c r="O61" s="30"/>
     </row>
     <row r="62" spans="2:15" s="17" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="43" t="s">
+      <c r="B62" s="44" t="s">
         <v>138</v>
       </c>
-      <c r="C62" s="43"/>
-      <c r="D62" s="43"/>
-      <c r="E62" s="43"/>
-      <c r="F62" s="43"/>
-      <c r="G62" s="43"/>
-      <c r="H62" s="43"/>
-      <c r="I62" s="43"/>
-      <c r="J62" s="43"/>
-      <c r="K62" s="43"/>
-      <c r="L62" s="43"/>
-      <c r="M62" s="43"/>
-      <c r="N62" s="43"/>
+      <c r="C62" s="44"/>
+      <c r="D62" s="44"/>
+      <c r="E62" s="44"/>
+      <c r="F62" s="44"/>
+      <c r="G62" s="44"/>
+      <c r="H62" s="44"/>
+      <c r="I62" s="44"/>
+      <c r="J62" s="44"/>
+      <c r="K62" s="44"/>
+      <c r="L62" s="44"/>
+      <c r="M62" s="44"/>
+      <c r="N62" s="44"/>
       <c r="O62" s="30"/>
     </row>
     <row r="63" spans="2:15" s="17" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4423,7 +4429,7 @@
     </row>
     <row r="65" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B65" s="26" t="s">
-        <v>140</v>
+        <v>154</v>
       </c>
       <c r="C65" s="24" t="s">
         <v>37</v>
@@ -4453,7 +4459,7 @@
         <v>36</v>
       </c>
       <c r="L65" s="27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="M65" s="24" t="s">
         <v>16</v>
@@ -4465,10 +4471,10 @@
     </row>
     <row r="66" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B66" s="26" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C66" s="24" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="D66" s="24" t="s">
         <v>41</v>
@@ -4495,7 +4501,7 @@
         <v>36</v>
       </c>
       <c r="L66" s="27" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M66" s="24" t="s">
         <v>36</v>
@@ -4514,7 +4520,7 @@
         <v>1</v>
       </c>
       <c r="C68" s="37" t="s">
-        <v>242</v>
+        <v>266</v>
       </c>
       <c r="D68" s="18"/>
       <c r="E68" s="20"/>
@@ -4530,21 +4536,21 @@
       <c r="O68" s="30"/>
     </row>
     <row r="69" spans="2:15" s="17" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="43" t="s">
-        <v>144</v>
-      </c>
-      <c r="C69" s="43"/>
-      <c r="D69" s="43"/>
-      <c r="E69" s="43"/>
-      <c r="F69" s="43"/>
-      <c r="G69" s="43"/>
-      <c r="H69" s="43"/>
-      <c r="I69" s="43"/>
-      <c r="J69" s="43"/>
-      <c r="K69" s="43"/>
-      <c r="L69" s="43"/>
-      <c r="M69" s="43"/>
-      <c r="N69" s="43"/>
+      <c r="B69" s="44" t="s">
+        <v>143</v>
+      </c>
+      <c r="C69" s="44"/>
+      <c r="D69" s="44"/>
+      <c r="E69" s="44"/>
+      <c r="F69" s="44"/>
+      <c r="G69" s="44"/>
+      <c r="H69" s="44"/>
+      <c r="I69" s="44"/>
+      <c r="J69" s="44"/>
+      <c r="K69" s="44"/>
+      <c r="L69" s="44"/>
+      <c r="M69" s="44"/>
+      <c r="N69" s="44"/>
       <c r="O69" s="30"/>
     </row>
     <row r="70" spans="2:15" s="17" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4623,7 +4629,7 @@
         <v>16</v>
       </c>
       <c r="L71" s="27" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="M71" s="24" t="s">
         <v>16</v>
@@ -4635,7 +4641,7 @@
     </row>
     <row r="72" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B72" s="26" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="C72" s="24" t="s">
         <v>37</v>
@@ -4661,9 +4667,11 @@
       <c r="J72" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="K72" s="23"/>
+      <c r="K72" s="23" t="s">
+        <v>36</v>
+      </c>
       <c r="L72" s="27" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="M72" s="24" t="s">
         <v>16</v>
@@ -4675,10 +4683,10 @@
     </row>
     <row r="73" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B73" s="26" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C73" s="24" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="D73" s="24" t="s">
         <v>41</v>
@@ -4701,9 +4709,11 @@
       <c r="J73" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="K73" s="23"/>
+      <c r="K73" s="23" t="s">
+        <v>36</v>
+      </c>
       <c r="L73" s="27" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M73" s="24" t="s">
         <v>36</v>
@@ -4722,7 +4732,7 @@
         <v>1</v>
       </c>
       <c r="C75" s="37" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="D75" s="18"/>
       <c r="E75" s="20"/>
@@ -4738,21 +4748,21 @@
       <c r="O75" s="30"/>
     </row>
     <row r="76" spans="2:15" s="17" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="43" t="s">
-        <v>148</v>
-      </c>
-      <c r="C76" s="43"/>
-      <c r="D76" s="43"/>
-      <c r="E76" s="43"/>
-      <c r="F76" s="43"/>
-      <c r="G76" s="43"/>
-      <c r="H76" s="43"/>
-      <c r="I76" s="43"/>
-      <c r="J76" s="43"/>
-      <c r="K76" s="43"/>
-      <c r="L76" s="43"/>
-      <c r="M76" s="43"/>
-      <c r="N76" s="43"/>
+      <c r="B76" s="44" t="s">
+        <v>147</v>
+      </c>
+      <c r="C76" s="44"/>
+      <c r="D76" s="44"/>
+      <c r="E76" s="44"/>
+      <c r="F76" s="44"/>
+      <c r="G76" s="44"/>
+      <c r="H76" s="44"/>
+      <c r="I76" s="44"/>
+      <c r="J76" s="44"/>
+      <c r="K76" s="44"/>
+      <c r="L76" s="44"/>
+      <c r="M76" s="44"/>
+      <c r="N76" s="44"/>
       <c r="O76" s="30"/>
     </row>
     <row r="77" spans="2:15" s="17" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4831,7 +4841,7 @@
         <v>16</v>
       </c>
       <c r="L78" s="27" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="M78" s="24" t="s">
         <v>16</v>
@@ -4864,7 +4874,7 @@
         <v>36</v>
       </c>
       <c r="I79" s="23" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="J79" s="23" t="s">
         <v>36</v>
@@ -4873,7 +4883,7 @@
         <v>36</v>
       </c>
       <c r="L79" s="27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="M79" s="24" t="s">
         <v>16</v>
@@ -4887,7 +4897,7 @@
     </row>
     <row r="80" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B80" s="26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C80" s="24" t="s">
         <v>47</v>
@@ -4917,16 +4927,16 @@
         <v>36</v>
       </c>
       <c r="L80" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="M80" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="N80" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="O80" s="31" t="s">
         <v>151</v>
-      </c>
-      <c r="M80" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="N80" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="O80" s="31" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="81" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -4950,7 +4960,7 @@
         <v>1</v>
       </c>
       <c r="C82" s="37" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="D82" s="18"/>
       <c r="E82" s="20"/>
@@ -4966,21 +4976,21 @@
       <c r="O82" s="30"/>
     </row>
     <row r="83" spans="2:15" s="17" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="43" t="s">
-        <v>153</v>
-      </c>
-      <c r="C83" s="43"/>
-      <c r="D83" s="43"/>
-      <c r="E83" s="43"/>
-      <c r="F83" s="43"/>
-      <c r="G83" s="43"/>
-      <c r="H83" s="43"/>
-      <c r="I83" s="43"/>
-      <c r="J83" s="43"/>
-      <c r="K83" s="43"/>
-      <c r="L83" s="43"/>
-      <c r="M83" s="43"/>
-      <c r="N83" s="43"/>
+      <c r="B83" s="44" t="s">
+        <v>152</v>
+      </c>
+      <c r="C83" s="44"/>
+      <c r="D83" s="44"/>
+      <c r="E83" s="44"/>
+      <c r="F83" s="44"/>
+      <c r="G83" s="44"/>
+      <c r="H83" s="44"/>
+      <c r="I83" s="44"/>
+      <c r="J83" s="44"/>
+      <c r="K83" s="44"/>
+      <c r="L83" s="44"/>
+      <c r="M83" s="44"/>
+      <c r="N83" s="44"/>
       <c r="O83" s="30"/>
     </row>
     <row r="84" spans="2:15" s="17" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5059,7 +5069,7 @@
         <v>16</v>
       </c>
       <c r="L85" s="27" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M85" s="24" t="s">
         <v>16</v>
@@ -5071,7 +5081,7 @@
     </row>
     <row r="86" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B86" s="26" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C86" s="24" t="s">
         <v>37</v>
@@ -5101,7 +5111,7 @@
         <v>36</v>
       </c>
       <c r="L86" s="27" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M86" s="24" t="s">
         <v>16</v>
@@ -5113,10 +5123,10 @@
     </row>
     <row r="87" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B87" s="26" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C87" s="24" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="D87" s="24" t="s">
         <v>41</v>
@@ -5143,7 +5153,7 @@
         <v>36</v>
       </c>
       <c r="L87" s="27" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="M87" s="24" t="s">
         <v>36</v>
@@ -5155,7 +5165,7 @@
     </row>
     <row r="88" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B88" s="26" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C88" s="24" t="s">
         <v>38</v>
@@ -5185,7 +5195,7 @@
         <v>36</v>
       </c>
       <c r="L88" s="27" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M88" s="24" t="s">
         <v>36</v>
@@ -5229,7 +5239,7 @@
         <v>36</v>
       </c>
       <c r="L89" s="27" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M89" s="24" t="s">
         <v>36</v>
@@ -5273,51 +5283,51 @@
         <v>36</v>
       </c>
       <c r="L90" s="27" t="s">
+        <v>160</v>
+      </c>
+      <c r="M90" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="N90" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="O90" s="40" t="s">
         <v>161</v>
-      </c>
-      <c r="M90" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="N90" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="O90" s="62" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="91" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B91" s="26" t="s">
+        <v>162</v>
+      </c>
+      <c r="C91" s="24" t="s">
+        <v>256</v>
+      </c>
+      <c r="D91" s="24">
+        <v>16</v>
+      </c>
+      <c r="E91" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="F91" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="G91" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="H91" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="I91" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="J91" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="K91" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="L91" s="27" t="s">
         <v>163</v>
-      </c>
-      <c r="C91" s="24" t="s">
-        <v>263</v>
-      </c>
-      <c r="D91" s="24">
-        <v>16</v>
-      </c>
-      <c r="E91" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="F91" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="G91" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="H91" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="I91" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="J91" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="K91" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="L91" s="27" t="s">
-        <v>164</v>
       </c>
       <c r="M91" s="24" t="s">
         <v>36</v>
@@ -5329,37 +5339,37 @@
     </row>
     <row r="92" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B92" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="C92" s="24" t="s">
+        <v>256</v>
+      </c>
+      <c r="D92" s="24">
+        <v>16</v>
+      </c>
+      <c r="E92" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="F92" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="G92" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="H92" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="I92" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="J92" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="K92" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="L92" s="27" t="s">
         <v>165</v>
-      </c>
-      <c r="C92" s="24" t="s">
-        <v>263</v>
-      </c>
-      <c r="D92" s="24">
-        <v>16</v>
-      </c>
-      <c r="E92" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="F92" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="G92" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="H92" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="I92" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="J92" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="K92" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="L92" s="27" t="s">
-        <v>166</v>
       </c>
       <c r="M92" s="24" t="s">
         <v>36</v>
@@ -5371,7 +5381,7 @@
     </row>
     <row r="93" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B93" s="26" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C93" s="24" t="s">
         <v>38</v>
@@ -5401,7 +5411,7 @@
         <v>36</v>
       </c>
       <c r="L93" s="27" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="M93" s="24" t="s">
         <v>36</v>
@@ -5415,7 +5425,7 @@
     </row>
     <row r="94" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B94" s="26" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C94" s="24" t="s">
         <v>38</v>
@@ -5445,7 +5455,7 @@
         <v>36</v>
       </c>
       <c r="L94" s="27" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="M94" s="24" t="s">
         <v>36</v>
@@ -5459,7 +5469,7 @@
     </row>
     <row r="95" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B95" s="26" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C95" s="24" t="s">
         <v>47</v>
@@ -5489,16 +5499,16 @@
         <v>36</v>
       </c>
       <c r="L95" s="27" t="s">
+        <v>171</v>
+      </c>
+      <c r="M95" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="N95" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="O95" s="31" t="s">
         <v>172</v>
-      </c>
-      <c r="M95" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="N95" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="O95" s="31" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="96" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -5510,7 +5520,7 @@
         <v>1</v>
       </c>
       <c r="C97" s="37" t="s">
-        <v>245</v>
+        <v>267</v>
       </c>
       <c r="D97" s="18"/>
       <c r="E97" s="20"/>
@@ -5526,21 +5536,21 @@
       <c r="O97" s="30"/>
     </row>
     <row r="98" spans="2:15" s="17" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B98" s="43" t="s">
-        <v>174</v>
-      </c>
-      <c r="C98" s="43"/>
-      <c r="D98" s="43"/>
-      <c r="E98" s="43"/>
-      <c r="F98" s="43"/>
-      <c r="G98" s="43"/>
-      <c r="H98" s="43"/>
-      <c r="I98" s="43"/>
-      <c r="J98" s="43"/>
-      <c r="K98" s="43"/>
-      <c r="L98" s="43"/>
-      <c r="M98" s="43"/>
-      <c r="N98" s="43"/>
+      <c r="B98" s="44" t="s">
+        <v>173</v>
+      </c>
+      <c r="C98" s="44"/>
+      <c r="D98" s="44"/>
+      <c r="E98" s="44"/>
+      <c r="F98" s="44"/>
+      <c r="G98" s="44"/>
+      <c r="H98" s="44"/>
+      <c r="I98" s="44"/>
+      <c r="J98" s="44"/>
+      <c r="K98" s="44"/>
+      <c r="L98" s="44"/>
+      <c r="M98" s="44"/>
+      <c r="N98" s="44"/>
       <c r="O98" s="30"/>
     </row>
     <row r="99" spans="2:15" s="17" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5619,7 +5629,7 @@
         <v>16</v>
       </c>
       <c r="L100" s="27" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M100" s="24" t="s">
         <v>16</v>
@@ -5631,7 +5641,7 @@
     </row>
     <row r="101" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B101" s="26" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="C101" s="24" t="s">
         <v>37</v>
@@ -5661,7 +5671,7 @@
         <v>36</v>
       </c>
       <c r="L101" s="27" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M101" s="24" t="s">
         <v>16</v>
@@ -5673,7 +5683,7 @@
     </row>
     <row r="102" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B102" s="26" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="C102" s="24" t="s">
         <v>37</v>
@@ -5703,7 +5713,7 @@
         <v>36</v>
       </c>
       <c r="L102" s="27" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="M102" s="24" t="s">
         <v>36</v>
@@ -5715,7 +5725,7 @@
     </row>
     <row r="103" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B103" s="26" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C103" s="24" t="s">
         <v>48</v>
@@ -5745,7 +5755,7 @@
         <v>36</v>
       </c>
       <c r="L103" s="27" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M103" s="24" t="s">
         <v>36</v>
@@ -5757,7 +5767,7 @@
     </row>
     <row r="104" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B104" s="26" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C104" s="24" t="s">
         <v>38</v>
@@ -5787,7 +5797,7 @@
         <v>36</v>
       </c>
       <c r="L104" s="27" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M104" s="24" t="s">
         <v>36</v>
@@ -5801,7 +5811,7 @@
     </row>
     <row r="105" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B105" s="26" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="C105" s="24" t="s">
         <v>47</v>
@@ -5831,7 +5841,7 @@
         <v>36</v>
       </c>
       <c r="L105" s="27" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M105" s="24" t="s">
         <v>36</v>
@@ -5852,7 +5862,7 @@
         <v>1</v>
       </c>
       <c r="C107" s="37" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="D107" s="18"/>
       <c r="E107" s="20"/>
@@ -5868,21 +5878,21 @@
       <c r="O107" s="30"/>
     </row>
     <row r="108" spans="2:15" s="17" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B108" s="43" t="s">
-        <v>181</v>
-      </c>
-      <c r="C108" s="43"/>
-      <c r="D108" s="43"/>
-      <c r="E108" s="43"/>
-      <c r="F108" s="43"/>
-      <c r="G108" s="43"/>
-      <c r="H108" s="43"/>
-      <c r="I108" s="43"/>
-      <c r="J108" s="43"/>
-      <c r="K108" s="43"/>
-      <c r="L108" s="43"/>
-      <c r="M108" s="43"/>
-      <c r="N108" s="43"/>
+      <c r="B108" s="44" t="s">
+        <v>180</v>
+      </c>
+      <c r="C108" s="44"/>
+      <c r="D108" s="44"/>
+      <c r="E108" s="44"/>
+      <c r="F108" s="44"/>
+      <c r="G108" s="44"/>
+      <c r="H108" s="44"/>
+      <c r="I108" s="44"/>
+      <c r="J108" s="44"/>
+      <c r="K108" s="44"/>
+      <c r="L108" s="44"/>
+      <c r="M108" s="44"/>
+      <c r="N108" s="44"/>
       <c r="O108" s="30"/>
     </row>
     <row r="109" spans="2:15" s="17" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5961,7 +5971,7 @@
         <v>16</v>
       </c>
       <c r="L110" s="27" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M110" s="24" t="s">
         <v>16</v>
@@ -5973,7 +5983,7 @@
     </row>
     <row r="111" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B111" s="26" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C111" s="24" t="s">
         <v>38</v>
@@ -6003,7 +6013,7 @@
         <v>36</v>
       </c>
       <c r="L111" s="27" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="M111" s="24" t="s">
         <v>36</v>
@@ -6047,7 +6057,7 @@
         <v>36</v>
       </c>
       <c r="L112" s="27" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M112" s="24" t="s">
         <v>36</v>
@@ -6056,12 +6066,12 @@
         <v>36</v>
       </c>
       <c r="O112" s="24" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="113" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B113" s="26" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C113" s="24" t="s">
         <v>47</v>
@@ -6091,21 +6101,21 @@
         <v>36</v>
       </c>
       <c r="L113" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="M113" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="N113" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="O113" s="31" t="s">
         <v>187</v>
-      </c>
-      <c r="M113" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="N113" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="O113" s="31" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="114" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B114" s="26" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C114" s="24" t="s">
         <v>47</v>
@@ -6135,16 +6145,16 @@
         <v>36</v>
       </c>
       <c r="L114" s="27" t="s">
+        <v>189</v>
+      </c>
+      <c r="M114" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="N114" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="O114" s="31" t="s">
         <v>190</v>
-      </c>
-      <c r="M114" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="N114" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="O114" s="31" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="115" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -6156,7 +6166,7 @@
         <v>1</v>
       </c>
       <c r="C116" s="37" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="D116" s="18"/>
       <c r="E116" s="20"/>
@@ -6172,21 +6182,21 @@
       <c r="O116" s="30"/>
     </row>
     <row r="117" spans="2:15" s="17" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B117" s="43" t="s">
-        <v>192</v>
-      </c>
-      <c r="C117" s="43"/>
-      <c r="D117" s="43"/>
-      <c r="E117" s="43"/>
-      <c r="F117" s="43"/>
-      <c r="G117" s="43"/>
-      <c r="H117" s="43"/>
-      <c r="I117" s="43"/>
-      <c r="J117" s="43"/>
-      <c r="K117" s="43"/>
-      <c r="L117" s="43"/>
-      <c r="M117" s="43"/>
-      <c r="N117" s="43"/>
+      <c r="B117" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="C117" s="44"/>
+      <c r="D117" s="44"/>
+      <c r="E117" s="44"/>
+      <c r="F117" s="44"/>
+      <c r="G117" s="44"/>
+      <c r="H117" s="44"/>
+      <c r="I117" s="44"/>
+      <c r="J117" s="44"/>
+      <c r="K117" s="44"/>
+      <c r="L117" s="44"/>
+      <c r="M117" s="44"/>
+      <c r="N117" s="44"/>
       <c r="O117" s="30"/>
     </row>
     <row r="118" spans="2:15" s="17" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6265,7 +6275,7 @@
         <v>16</v>
       </c>
       <c r="L119" s="27" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="M119" s="24" t="s">
         <v>16</v>
@@ -6277,7 +6287,7 @@
     </row>
     <row r="120" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B120" s="26" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C120" s="24" t="s">
         <v>37</v>
@@ -6307,7 +6317,7 @@
         <v>36</v>
       </c>
       <c r="L120" s="27" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="M120" s="24" t="s">
         <v>36</v>
@@ -6349,7 +6359,7 @@
         <v>36</v>
       </c>
       <c r="L121" s="27" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="M121" s="24" t="s">
         <v>36</v>
@@ -6358,12 +6368,12 @@
         <v>36</v>
       </c>
       <c r="O121" s="24" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="122" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B122" s="26" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C122" s="24" t="s">
         <v>38</v>
@@ -6393,7 +6403,7 @@
         <v>36</v>
       </c>
       <c r="L122" s="27" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="M122" s="24" t="s">
         <v>36</v>
@@ -6407,7 +6417,7 @@
     </row>
     <row r="123" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B123" s="26" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C123" s="24" t="s">
         <v>37</v>
@@ -6437,7 +6447,7 @@
         <v>36</v>
       </c>
       <c r="L123" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="M123" s="24" t="s">
         <v>36</v>
@@ -6449,7 +6459,7 @@
     </row>
     <row r="124" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B124" s="26" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="C124" s="24" t="s">
         <v>47</v>
@@ -6479,21 +6489,21 @@
         <v>36</v>
       </c>
       <c r="L124" s="27" t="s">
+        <v>200</v>
+      </c>
+      <c r="M124" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="N124" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="O124" s="31" t="s">
         <v>201</v>
-      </c>
-      <c r="M124" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="N124" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="O124" s="31" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="125" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B125" s="26" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="C125" s="24" t="s">
         <v>47</v>
@@ -6523,7 +6533,7 @@
         <v>36</v>
       </c>
       <c r="L125" s="27" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="M125" s="24" t="s">
         <v>36</v>
@@ -6532,12 +6542,12 @@
         <v>16</v>
       </c>
       <c r="O125" s="31" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="126" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B126" s="26" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C126" s="24" t="s">
         <v>47</v>
@@ -6567,16 +6577,16 @@
         <v>36</v>
       </c>
       <c r="L126" s="27" t="s">
+        <v>204</v>
+      </c>
+      <c r="M126" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="N126" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="O126" s="31" t="s">
         <v>205</v>
-      </c>
-      <c r="M126" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="N126" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="O126" s="31" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="127" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -6588,7 +6598,7 @@
         <v>1</v>
       </c>
       <c r="C128" s="37" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="D128" s="18"/>
       <c r="E128" s="20"/>
@@ -6604,21 +6614,21 @@
       <c r="O128" s="30"/>
     </row>
     <row r="129" spans="2:15" s="17" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B129" s="43" t="s">
-        <v>207</v>
-      </c>
-      <c r="C129" s="43"/>
-      <c r="D129" s="43"/>
-      <c r="E129" s="43"/>
-      <c r="F129" s="43"/>
-      <c r="G129" s="43"/>
-      <c r="H129" s="43"/>
-      <c r="I129" s="43"/>
-      <c r="J129" s="43"/>
-      <c r="K129" s="43"/>
-      <c r="L129" s="43"/>
-      <c r="M129" s="43"/>
-      <c r="N129" s="43"/>
+      <c r="B129" s="44" t="s">
+        <v>206</v>
+      </c>
+      <c r="C129" s="44"/>
+      <c r="D129" s="44"/>
+      <c r="E129" s="44"/>
+      <c r="F129" s="44"/>
+      <c r="G129" s="44"/>
+      <c r="H129" s="44"/>
+      <c r="I129" s="44"/>
+      <c r="J129" s="44"/>
+      <c r="K129" s="44"/>
+      <c r="L129" s="44"/>
+      <c r="M129" s="44"/>
+      <c r="N129" s="44"/>
       <c r="O129" s="30"/>
     </row>
     <row r="130" spans="2:15" s="17" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6697,7 +6707,7 @@
         <v>16</v>
       </c>
       <c r="L131" s="27" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="M131" s="24" t="s">
         <v>16</v>
@@ -6709,7 +6719,7 @@
     </row>
     <row r="132" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B132" s="26" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C132" s="24" t="s">
         <v>37</v>
@@ -6739,7 +6749,7 @@
         <v>36</v>
       </c>
       <c r="L132" s="27" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="M132" s="24" t="s">
         <v>36</v>
@@ -6751,7 +6761,7 @@
     </row>
     <row r="133" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B133" s="26" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C133" s="24" t="s">
         <v>37</v>
@@ -6781,7 +6791,7 @@
         <v>36</v>
       </c>
       <c r="L133" s="27" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="M133" s="24" t="s">
         <v>36</v>
@@ -6796,7 +6806,7 @@
         <v>127</v>
       </c>
       <c r="C134" s="24" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="D134" s="24">
         <v>16</v>
@@ -6823,7 +6833,7 @@
         <v>36</v>
       </c>
       <c r="L134" s="27" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="M134" s="24" t="s">
         <v>36</v>
@@ -6832,7 +6842,7 @@
         <v>36</v>
       </c>
       <c r="O134" s="24" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
     </row>
     <row r="135" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -6867,7 +6877,7 @@
         <v>36</v>
       </c>
       <c r="L135" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="M135" s="24" t="s">
         <v>36</v>
@@ -6876,12 +6886,12 @@
         <v>36</v>
       </c>
       <c r="O135" s="24" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="136" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B136" s="26" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C136" s="24" t="s">
         <v>38</v>
@@ -6911,7 +6921,7 @@
         <v>36</v>
       </c>
       <c r="L136" s="27" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="M136" s="24" t="s">
         <v>36</v>
@@ -6925,7 +6935,7 @@
     </row>
     <row r="137" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B137" s="26" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C137" s="24" t="s">
         <v>38</v>
@@ -6955,7 +6965,7 @@
         <v>36</v>
       </c>
       <c r="L137" s="27" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="M137" s="24" t="s">
         <v>36</v>
@@ -6969,7 +6979,7 @@
     </row>
     <row r="138" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B138" s="26" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C138" s="24" t="s">
         <v>47</v>
@@ -6999,16 +7009,16 @@
         <v>36</v>
       </c>
       <c r="L138" s="27" t="s">
+        <v>214</v>
+      </c>
+      <c r="M138" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="N138" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="O138" s="31" t="s">
         <v>215</v>
-      </c>
-      <c r="M138" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="N138" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="O138" s="31" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="139" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -7020,7 +7030,7 @@
         <v>1</v>
       </c>
       <c r="C140" s="37" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D140" s="18"/>
       <c r="E140" s="20"/>
@@ -7036,21 +7046,21 @@
       <c r="O140" s="30"/>
     </row>
     <row r="141" spans="2:15" s="17" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B141" s="43" t="s">
-        <v>218</v>
-      </c>
-      <c r="C141" s="43"/>
-      <c r="D141" s="43"/>
-      <c r="E141" s="43"/>
-      <c r="F141" s="43"/>
-      <c r="G141" s="43"/>
-      <c r="H141" s="43"/>
-      <c r="I141" s="43"/>
-      <c r="J141" s="43"/>
-      <c r="K141" s="43"/>
-      <c r="L141" s="43"/>
-      <c r="M141" s="43"/>
-      <c r="N141" s="43"/>
+      <c r="B141" s="44" t="s">
+        <v>217</v>
+      </c>
+      <c r="C141" s="44"/>
+      <c r="D141" s="44"/>
+      <c r="E141" s="44"/>
+      <c r="F141" s="44"/>
+      <c r="G141" s="44"/>
+      <c r="H141" s="44"/>
+      <c r="I141" s="44"/>
+      <c r="J141" s="44"/>
+      <c r="K141" s="44"/>
+      <c r="L141" s="44"/>
+      <c r="M141" s="44"/>
+      <c r="N141" s="44"/>
       <c r="O141" s="30"/>
     </row>
     <row r="142" spans="2:15" s="17" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7129,7 +7139,7 @@
         <v>16</v>
       </c>
       <c r="L143" s="27" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M143" s="24" t="s">
         <v>16</v>
@@ -7141,7 +7151,7 @@
     </row>
     <row r="144" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B144" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C144" s="24" t="s">
         <v>37</v>
@@ -7171,7 +7181,7 @@
         <v>36</v>
       </c>
       <c r="L144" s="27" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="M144" s="24" t="s">
         <v>16</v>
@@ -7183,7 +7193,7 @@
     </row>
     <row r="145" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B145" s="26" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C145" s="24" t="s">
         <v>82</v>
@@ -7213,7 +7223,7 @@
         <v>36</v>
       </c>
       <c r="L145" s="27" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M145" s="24" t="s">
         <v>36</v>
@@ -7222,12 +7232,12 @@
         <v>36</v>
       </c>
       <c r="O145" s="31" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
     </row>
     <row r="146" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B146" s="26" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C146" s="24" t="s">
         <v>38</v>
@@ -7257,7 +7267,7 @@
         <v>36</v>
       </c>
       <c r="L146" s="27" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="M146" s="24" t="s">
         <v>36</v>
@@ -7271,7 +7281,7 @@
     </row>
     <row r="147" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B147" s="26" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C147" s="24" t="s">
         <v>39</v>
@@ -7301,7 +7311,7 @@
         <v>36</v>
       </c>
       <c r="L147" s="27" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M147" s="24" t="s">
         <v>36</v>
@@ -7345,16 +7355,16 @@
         <v>36</v>
       </c>
       <c r="L148" s="27" t="s">
+        <v>226</v>
+      </c>
+      <c r="M148" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="N148" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="O148" s="31" t="s">
         <v>227</v>
-      </c>
-      <c r="M148" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="N148" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="O148" s="31" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="149" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -7366,7 +7376,7 @@
         <v>1</v>
       </c>
       <c r="C150" s="37" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="D150" s="18"/>
       <c r="E150" s="20"/>
@@ -7382,21 +7392,21 @@
       <c r="O150" s="30"/>
     </row>
     <row r="151" spans="2:15" s="17" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B151" s="43" t="s">
-        <v>229</v>
-      </c>
-      <c r="C151" s="43"/>
-      <c r="D151" s="43"/>
-      <c r="E151" s="43"/>
-      <c r="F151" s="43"/>
-      <c r="G151" s="43"/>
-      <c r="H151" s="43"/>
-      <c r="I151" s="43"/>
-      <c r="J151" s="43"/>
-      <c r="K151" s="43"/>
-      <c r="L151" s="43"/>
-      <c r="M151" s="43"/>
-      <c r="N151" s="43"/>
+      <c r="B151" s="44" t="s">
+        <v>228</v>
+      </c>
+      <c r="C151" s="44"/>
+      <c r="D151" s="44"/>
+      <c r="E151" s="44"/>
+      <c r="F151" s="44"/>
+      <c r="G151" s="44"/>
+      <c r="H151" s="44"/>
+      <c r="I151" s="44"/>
+      <c r="J151" s="44"/>
+      <c r="K151" s="44"/>
+      <c r="L151" s="44"/>
+      <c r="M151" s="44"/>
+      <c r="N151" s="44"/>
       <c r="O151" s="30"/>
     </row>
     <row r="152" spans="2:15" s="17" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7475,7 +7485,7 @@
         <v>16</v>
       </c>
       <c r="L153" s="27" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="M153" s="24" t="s">
         <v>16</v>
@@ -7487,7 +7497,7 @@
     </row>
     <row r="154" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B154" s="26" t="s">
-        <v>231</v>
+        <v>268</v>
       </c>
       <c r="C154" s="24" t="s">
         <v>38</v>
@@ -7517,7 +7527,7 @@
         <v>36</v>
       </c>
       <c r="L154" s="27" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="M154" s="24" t="s">
         <v>36</v>
@@ -7531,7 +7541,7 @@
     </row>
     <row r="155" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B155" s="26" t="s">
-        <v>233</v>
+        <v>269</v>
       </c>
       <c r="C155" s="24" t="s">
         <v>39</v>
@@ -7561,7 +7571,7 @@
         <v>36</v>
       </c>
       <c r="L155" s="27" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="M155" s="24" t="s">
         <v>36</v>
@@ -7575,7 +7585,7 @@
     </row>
     <row r="156" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B156" s="26" t="s">
-        <v>235</v>
+        <v>270</v>
       </c>
       <c r="C156" s="24" t="s">
         <v>38</v>
@@ -7605,7 +7615,7 @@
         <v>36</v>
       </c>
       <c r="L156" s="27" t="s">
-        <v>232</v>
+        <v>265</v>
       </c>
       <c r="M156" s="24" t="s">
         <v>36</v>
@@ -7619,7 +7629,7 @@
     </row>
     <row r="157" spans="2:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B157" s="26" t="s">
-        <v>236</v>
+        <v>271</v>
       </c>
       <c r="C157" s="24" t="s">
         <v>39</v>
@@ -7649,7 +7659,7 @@
         <v>36</v>
       </c>
       <c r="L157" s="27" t="s">
-        <v>234</v>
+        <v>264</v>
       </c>
       <c r="M157" s="24" t="s">
         <v>36</v>
@@ -7665,7 +7675,7 @@
       <c r="B158" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="C158" s="24" t="s">
+      <c r="C158" s="63" t="s">
         <v>47</v>
       </c>
       <c r="D158" s="24">
@@ -7693,7 +7703,7 @@
         <v>36</v>
       </c>
       <c r="L158" s="27" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="M158" s="24" t="s">
         <v>16</v>
@@ -7702,7 +7712,7 @@
         <v>16</v>
       </c>
       <c r="O158" s="31" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -7770,30 +7780,30 @@
       <c r="O2" s="30"/>
     </row>
     <row r="3" spans="2:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="43"/>
-      <c r="N3" s="43"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="44"/>
       <c r="O3" s="30"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="54" t="s">
+      <c r="B4" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="55"/>
-      <c r="D4" s="54" t="s">
+      <c r="C4" s="56"/>
+      <c r="D4" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="55"/>
+      <c r="E4" s="56"/>
       <c r="F4" s="22"/>
       <c r="G4" s="22"/>
       <c r="H4" s="22"/>
@@ -7818,128 +7828,128 @@
       <c r="E5" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="F5" s="56"/>
-      <c r="G5" s="57"/>
-      <c r="H5" s="57"/>
-      <c r="I5" s="57"/>
-      <c r="J5" s="57"/>
-      <c r="K5" s="57"/>
-      <c r="L5" s="57"/>
-      <c r="M5" s="57"/>
-      <c r="N5" s="57"/>
-      <c r="O5" s="58"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="58"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="58"/>
+      <c r="K5" s="58"/>
+      <c r="L5" s="58"/>
+      <c r="M5" s="58"/>
+      <c r="N5" s="58"/>
+      <c r="O5" s="59"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="24"/>
       <c r="C6" s="24"/>
       <c r="D6" s="24"/>
       <c r="E6" s="24"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="46"/>
-      <c r="K6" s="46"/>
-      <c r="L6" s="46"/>
-      <c r="M6" s="46"/>
-      <c r="N6" s="46"/>
-      <c r="O6" s="47"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="47"/>
+      <c r="N6" s="47"/>
+      <c r="O6" s="48"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="26"/>
       <c r="C7" s="24"/>
       <c r="D7" s="24"/>
       <c r="E7" s="23"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="46"/>
-      <c r="J7" s="46"/>
-      <c r="K7" s="46"/>
-      <c r="L7" s="46"/>
-      <c r="M7" s="46"/>
-      <c r="N7" s="46"/>
-      <c r="O7" s="47"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="47"/>
+      <c r="J7" s="47"/>
+      <c r="K7" s="47"/>
+      <c r="L7" s="47"/>
+      <c r="M7" s="47"/>
+      <c r="N7" s="47"/>
+      <c r="O7" s="48"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" s="26"/>
       <c r="C8" s="24"/>
       <c r="D8" s="24"/>
       <c r="E8" s="23"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="60"/>
-      <c r="H8" s="60"/>
-      <c r="I8" s="60"/>
-      <c r="J8" s="60"/>
-      <c r="K8" s="60"/>
-      <c r="L8" s="60"/>
-      <c r="M8" s="60"/>
-      <c r="N8" s="60"/>
-      <c r="O8" s="61"/>
+      <c r="F8" s="60"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="61"/>
+      <c r="I8" s="61"/>
+      <c r="J8" s="61"/>
+      <c r="K8" s="61"/>
+      <c r="L8" s="61"/>
+      <c r="M8" s="61"/>
+      <c r="N8" s="61"/>
+      <c r="O8" s="62"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" s="26"/>
       <c r="C9" s="24"/>
       <c r="D9" s="24"/>
       <c r="E9" s="23"/>
-      <c r="F9" s="45"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="46"/>
-      <c r="J9" s="46"/>
-      <c r="K9" s="46"/>
-      <c r="L9" s="46"/>
-      <c r="M9" s="46"/>
-      <c r="N9" s="46"/>
-      <c r="O9" s="47"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="47"/>
+      <c r="J9" s="47"/>
+      <c r="K9" s="47"/>
+      <c r="L9" s="47"/>
+      <c r="M9" s="47"/>
+      <c r="N9" s="47"/>
+      <c r="O9" s="48"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" s="26"/>
       <c r="C10" s="24"/>
       <c r="D10" s="24"/>
       <c r="E10" s="23"/>
-      <c r="F10" s="45"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="46"/>
-      <c r="J10" s="46"/>
-      <c r="K10" s="46"/>
-      <c r="L10" s="46"/>
-      <c r="M10" s="46"/>
-      <c r="N10" s="46"/>
-      <c r="O10" s="47"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="47"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="47"/>
+      <c r="L10" s="47"/>
+      <c r="M10" s="47"/>
+      <c r="N10" s="47"/>
+      <c r="O10" s="48"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" s="26"/>
       <c r="C11" s="24"/>
       <c r="D11" s="24"/>
       <c r="E11" s="23"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="49"/>
-      <c r="H11" s="49"/>
-      <c r="I11" s="49"/>
-      <c r="J11" s="49"/>
-      <c r="K11" s="49"/>
-      <c r="L11" s="49"/>
-      <c r="M11" s="49"/>
-      <c r="N11" s="49"/>
-      <c r="O11" s="50"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="50"/>
+      <c r="L11" s="50"/>
+      <c r="M11" s="50"/>
+      <c r="N11" s="50"/>
+      <c r="O11" s="51"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" s="26"/>
       <c r="C12" s="24"/>
       <c r="D12" s="24"/>
       <c r="E12" s="23"/>
-      <c r="F12" s="51"/>
-      <c r="G12" s="52"/>
-      <c r="H12" s="52"/>
-      <c r="I12" s="52"/>
-      <c r="J12" s="52"/>
-      <c r="K12" s="52"/>
-      <c r="L12" s="52"/>
-      <c r="M12" s="52"/>
-      <c r="N12" s="52"/>
-      <c r="O12" s="53"/>
+      <c r="F12" s="52"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="53"/>
+      <c r="I12" s="53"/>
+      <c r="J12" s="53"/>
+      <c r="K12" s="53"/>
+      <c r="L12" s="53"/>
+      <c r="M12" s="53"/>
+      <c r="N12" s="53"/>
+      <c r="O12" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="11">

</xml_diff>